<commit_message>
After Mark's comments fixes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,72 +14,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>ot1</t>
+  </si>
+  <si>
+    <t>ot2</t>
+  </si>
+  <si>
+    <t>ot3</t>
+  </si>
+  <si>
+    <t>rp1</t>
+  </si>
+  <si>
+    <t>rp2</t>
+  </si>
+  <si>
+    <t>rt1</t>
+  </si>
+  <si>
+    <t>rt2</t>
+  </si>
+  <si>
+    <t>rt3</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>ft1</t>
+  </si>
+  <si>
+    <t>ft2</t>
+  </si>
   <si>
     <t>discuss_rank</t>
   </si>
   <si>
-    <t>f1</t>
-  </si>
-  <si>
-    <t>f3</t>
-  </si>
-  <si>
-    <t>ft1</t>
-  </si>
-  <si>
-    <t>ft2</t>
-  </si>
-  <si>
     <t>h_index</t>
   </si>
   <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
     <t>original_tweets</t>
   </si>
   <si>
-    <t>ot1</t>
-  </si>
-  <si>
-    <t>ot2</t>
-  </si>
-  <si>
-    <t>ot3</t>
-  </si>
-  <si>
-    <t>rp1</t>
-  </si>
-  <si>
-    <t>rp2</t>
-  </si>
-  <si>
-    <t>rt1</t>
-  </si>
-  <si>
-    <t>rt2</t>
-  </si>
-  <si>
-    <t>rt3</t>
-  </si>
-  <si>
     <t>spread_rank</t>
   </si>
   <si>
     <t>topical_signal</t>
   </si>
   <si>
-    <t>USER</t>
-  </si>
-  <si>
-    <t>netanyahu</t>
-  </si>
-  <si>
-    <t>Tzipi_Livni</t>
+    <t>mention_impact</t>
+  </si>
+  <si>
+    <t>social_networking_potential</t>
+  </si>
+  <si>
+    <t>popularity</t>
+  </si>
+  <si>
+    <t>interactor_ratio</t>
+  </si>
+  <si>
+    <t>signal_strength</t>
+  </si>
+  <si>
+    <t>tweet_count_score</t>
+  </si>
+  <si>
+    <t>activity_score</t>
+  </si>
+  <si>
+    <t>general_activity</t>
+  </si>
+  <si>
+    <t>retweet_impact</t>
+  </si>
+  <si>
+    <t>retweet_mention_ratio</t>
+  </si>
+  <si>
+    <t>follower_rank</t>
+  </si>
+  <si>
+    <t>yaniv33martin</t>
   </si>
 </sst>
 </file>
@@ -428,7 +464,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +472,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,129 +533,145 @@
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" t="n">
-        <v>0</v>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" t="n">
-        <v>971233</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>496</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>496</v>
+        <v>6</v>
       </c>
       <c r="K2" t="n">
-        <v>236</v>
+        <v>9</v>
       </c>
       <c r="L2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="M2" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>457</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>11</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9975212478233336</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
         <v>1</v>
       </c>
-      <c r="O2" t="n">
-        <v>49</v>
-      </c>
-      <c r="P2" t="n">
-        <v>568410</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>25842.02721774194</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.01788721757960003</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
-        <v>56641</v>
-      </c>
-      <c r="C3" t="n">
-        <v>102</v>
-      </c>
-      <c r="D3" t="n">
-        <v>292</v>
-      </c>
-      <c r="E3" t="n">
-        <v>560</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" t="n">
-        <v>109</v>
-      </c>
-      <c r="H3" t="n">
-        <v>70</v>
-      </c>
-      <c r="I3" t="n">
-        <v>560</v>
-      </c>
-      <c r="J3" t="n">
-        <v>560</v>
-      </c>
-      <c r="K3" t="n">
-        <v>264</v>
-      </c>
-      <c r="L3" t="n">
-        <v>13</v>
-      </c>
-      <c r="M3" t="n">
-        <v>54</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1</v>
-      </c>
-      <c r="O3" t="n">
-        <v>344</v>
-      </c>
-      <c r="P3" t="n">
-        <v>6168</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>261.9367231638418</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.037100240536197</v>
-      </c>
-      <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
-        <v>21</v>
+      <c r="AB2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>480</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Version - rp2 fixed
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>USER</t>
   </si>
@@ -115,7 +115,10 @@
     <t>follower_rank</t>
   </si>
   <si>
-    <t>StavShaffir</t>
+    <t>ishmuli</t>
+  </si>
+  <si>
+    <t>yaniv33martin</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -578,100 +581,201 @@
         <v>33</v>
       </c>
       <c r="B2" t="n">
-        <v>377</v>
+        <v>530</v>
       </c>
       <c r="C2" t="n">
-        <v>258</v>
+        <v>363</v>
       </c>
       <c r="D2" t="n">
         <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>188</v>
+        <v>407</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>520</v>
       </c>
       <c r="G2" t="n">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="H2" t="n">
-        <v>3428</v>
+        <v>1325</v>
       </c>
       <c r="I2" t="n">
-        <v>205.04350132626</v>
+        <v>76.22130102040816</v>
       </c>
       <c r="J2" t="n">
-        <v>112006</v>
+        <v>17495</v>
       </c>
       <c r="K2" t="n">
-        <v>648</v>
+        <v>795</v>
       </c>
       <c r="L2" t="n">
-        <v>55</v>
+        <v>170</v>
       </c>
       <c r="M2" t="n">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="N2" t="n">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="O2" t="n">
         <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>3118</v>
+        <v>5510</v>
       </c>
       <c r="Q2" t="n">
-        <v>377</v>
+        <v>525</v>
       </c>
       <c r="R2" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>377</v>
+        <v>530</v>
       </c>
       <c r="U2" t="n">
-        <v>0.01437000835123137</v>
+        <v>0.009435015273420415</v>
       </c>
       <c r="V2" t="n">
-        <v>0.008323424494649227</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>-87.50855338645745</v>
+        <v>-321.6560824573816</v>
       </c>
       <c r="X2" t="n">
-        <v>4.500919787785147</v>
+        <v>1.002206953444424</v>
       </c>
       <c r="Y2" t="n">
         <v>1</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.001839575570293198</v>
+        <v>0.004413906888848709</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>653</v>
+        <v>780</v>
       </c>
       <c r="AC2" t="n">
-        <v>113495</v>
+        <v>19477</v>
       </c>
       <c r="AD2" t="n">
-        <v>3959</v>
+        <v>6697</v>
       </c>
       <c r="AE2" t="n">
-        <v>3428</v>
+        <v>1325</v>
       </c>
       <c r="AF2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.9565336249316566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6</v>
+      </c>
+      <c r="K3" t="n">
         <v>9</v>
       </c>
-      <c r="AG2" t="n">
-        <v>0.9942478740213396</v>
+      <c r="L3" t="n">
+        <v>11</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>457</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>11</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.9975212478233336</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>38</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>480</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>